<commit_message>
updated contact page and added hover on navbar
</commit_message>
<xml_diff>
--- a/PlanningProject1.xlsx
+++ b/PlanningProject1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCR School\Project1\project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83C185BE-0AF7-4F76-93C6-99B4567DD618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EAA3CF-527C-4128-99AE-91F626B6AD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8EABCB6B-156C-49B5-B412-CA84D0997D9E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planning" sheetId="1" r:id="rId1"/>
+    <sheet name="Requirement list" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,70 +35,205 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
   <si>
     <t>Planning project</t>
   </si>
   <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Week 5</t>
-  </si>
-  <si>
-    <t>Week 6</t>
-  </si>
-  <si>
-    <t>Week 7</t>
-  </si>
-  <si>
-    <t>Week 8</t>
-  </si>
-  <si>
-    <t>Week 9</t>
-  </si>
-  <si>
     <t>Ik was tijdens de introductieweek niet aanwezig</t>
   </si>
   <si>
-    <t>Begin maken aan de website: pagina opmaak en layout, GitHub opzetten en planning maken</t>
-  </si>
-  <si>
-    <t>Begin maken aan de WireFrames en interviewdocument, website verder opvullen</t>
-  </si>
-  <si>
-    <t>CSS bestand aanmaken voor wat general styling, planning bijwerken waar nodig</t>
-  </si>
-  <si>
-    <t>Beginnen met images en video's in de website zetten</t>
-  </si>
-  <si>
-    <t>Relevante informatie toevoegen aan de website, anders Lorem Ipsum</t>
-  </si>
-  <si>
-    <t>Finishing touches op de website en kijken of alles goed werkt</t>
-  </si>
-  <si>
-    <t>Alle requirements doornemen en kijken of mijn website eraan voldoet</t>
-  </si>
-  <si>
-    <t>Presentatie</t>
+    <t>04-09 t/m 10-09</t>
+  </si>
+  <si>
+    <t>11-09 t/m 17-09</t>
+  </si>
+  <si>
+    <t>18-09 t/m 24-09</t>
+  </si>
+  <si>
+    <t>25-09 t/m 01-10</t>
+  </si>
+  <si>
+    <t>02-10 t/m 08-10</t>
+  </si>
+  <si>
+    <t>09-10 t/m 15-10</t>
+  </si>
+  <si>
+    <t>23-10 t/m 29-10</t>
+  </si>
+  <si>
+    <t>16-10 t/m 22-10</t>
+  </si>
+  <si>
+    <t>Herfstvakantie, dus niets doen en relaxen!</t>
+  </si>
+  <si>
+    <t>Deadline van het project, project en bijbehorende documenten inleveren</t>
+  </si>
+  <si>
+    <t>Introductieweek</t>
+  </si>
+  <si>
+    <t>Presentatie van het project portfolio aan minimaal 2 docenten</t>
+  </si>
+  <si>
+    <t>30-10 t/m 05-11</t>
+  </si>
+  <si>
+    <t>Analyse</t>
+  </si>
+  <si>
+    <t>Basisontwerp</t>
+  </si>
+  <si>
+    <t>Technisch ontwerp</t>
+  </si>
+  <si>
+    <t>Bouw</t>
+  </si>
+  <si>
+    <t>Testen</t>
+  </si>
+  <si>
+    <t>Integratie</t>
+  </si>
+  <si>
+    <t>Beheer</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Na het project</t>
+  </si>
+  <si>
+    <t>Website beheren en aanpassen waarbij nodig</t>
+  </si>
+  <si>
+    <t>Begin maken aan het project: planning maken, eisen doornemen en documenteren</t>
+  </si>
+  <si>
+    <t>Een sitemap maken met de WireFrame van de website en vorige taken afmaken als dat nodig is</t>
+  </si>
+  <si>
+    <t>HTML en CSS bestanden opmaken en aanvullen met een homepagina, een pagina met persoonlijke gegevens, een pagina met interviewvragen, een projectpagina en een contactpagina</t>
+  </si>
+  <si>
+    <t>Eisen in de websites implementeren: formulier in contactpagina, tabel in projectpagina en interviewpagina</t>
+  </si>
+  <si>
+    <t>Andere eisen implementeren: foto en video op persoonlijke pagina</t>
+  </si>
+  <si>
+    <t>Alle kopjes vullen met informatie en anders Lorem Ipsum als placeholder</t>
+  </si>
+  <si>
+    <t>Alle eisen doornemen en kijken of mijn website eraan voldoet en kijken of alle documentie in orde is</t>
+  </si>
+  <si>
+    <t>Eisen:</t>
+  </si>
+  <si>
+    <t>MoSCoW</t>
+  </si>
+  <si>
+    <t>De website bevat een homepagina en een pagina met informatie over wie je bent</t>
+  </si>
+  <si>
+    <t>De website maakt gebruik van de juiste HTML elementen</t>
+  </si>
+  <si>
+    <t>Elke webpagina bevat één keer de elementen DOCTYPE, html, head en body</t>
+  </si>
+  <si>
+    <t>De website is opgebouwd uit HTML en CSS</t>
+  </si>
+  <si>
+    <t>De opmaak van de website zit in een CSS-bestand</t>
+  </si>
+  <si>
+    <t>Er wordt geen gebruik gemaakt van de style-attribuut</t>
+  </si>
+  <si>
+    <t>Er wordt minimaal één foto geïmplementeerd in de website</t>
+  </si>
+  <si>
+    <t>Er wordt minimaal één video geïmplementeerd in de website</t>
+  </si>
+  <si>
+    <t>Er wordt minimaal één tabel met minimaal drie rijen geïmplementeerd in de website</t>
+  </si>
+  <si>
+    <t>Er wordt minimaal één formulier met drie inputs geïmplementeerd in de website</t>
+  </si>
+  <si>
+    <t>De website bevat een interview met minimaal vijf vragen met een medestudent</t>
+  </si>
+  <si>
+    <t>De website bevat een pagina met achtergrondinformatie: werkervaring en opleiding</t>
+  </si>
+  <si>
+    <t>De website bevat een pagina met projecten</t>
+  </si>
+  <si>
+    <t>De website bevat informatie over wat de developer kwijt wilt als student of software developer</t>
+  </si>
+  <si>
+    <t>De website bevat links naar social media</t>
+  </si>
+  <si>
+    <t>Website eisen:</t>
+  </si>
+  <si>
+    <t>Project eisen:</t>
+  </si>
+  <si>
+    <t>Het project bevat een WireFrame</t>
+  </si>
+  <si>
+    <t>Het project bevat een Sitemap</t>
+  </si>
+  <si>
+    <t>Het project bevat een planning</t>
+  </si>
+  <si>
+    <t>Het project bevat the MoSCoW methode</t>
+  </si>
+  <si>
+    <t>Overige eisen:</t>
+  </si>
+  <si>
+    <t>Het project bevat een functioneel ontwerp</t>
+  </si>
+  <si>
+    <t>Het project bevat een plan van aanpak</t>
+  </si>
+  <si>
+    <t>Het project bevat een plan van eisen</t>
+  </si>
+  <si>
+    <t>De code is gevalideerd</t>
+  </si>
+  <si>
+    <t>Must</t>
+  </si>
+  <si>
+    <t>03-11 23:59 uur</t>
+  </si>
+  <si>
+    <t>05-10 t/m 11-11</t>
+  </si>
+  <si>
+    <t>Project is af en voldaan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +248,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -121,7 +280,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -157,16 +316,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,158 +713,511 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39C3A13-15CB-47FD-92D5-CFC159B43958}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
     <col min="2" max="2" width="138.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="29.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7501C15D-395C-43E6-8608-4778C6105BF2}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="79.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="11"/>
+    </row>
+    <row r="3" spans="1:2" ht="36" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="36" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="36" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="36" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="36" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="36" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A18" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A22" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A24" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A26" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="11"/>
+    </row>
+    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>